<commit_message>
Branch and Line Coverage
</commit_message>
<xml_diff>
--- a/test/UnitTestSample.Test/Aula-05-TestCriteria/PCE-AVL-TD.xlsx
+++ b/test/UnitTestSample.Test/Aula-05-TestCriteria/PCE-AVL-TD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\mestrado\coo-299-18-testes\Aula-02-unit-test\test\UnitTestSample.Test\Aula-05-TestCriteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADED7CFD-9CB0-4300-B45A-B593A0D8424B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B075286-8F26-4C2E-8E1D-103FBCD06E57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{954EF424-EE12-4562-91A0-2A2C1669F98A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Nome</t>
   </si>
@@ -69,10 +69,13 @@
     <t>xUnit in line data</t>
   </si>
   <si>
-    <t>Argumento inválido</t>
-  </si>
-  <si>
     <t>Não é um cliente</t>
+  </si>
+  <si>
+    <t>Argumento inválido  (Parameter 'nome')</t>
+  </si>
+  <si>
+    <t>Argumento inválido  (Parameter 'idade')</t>
   </si>
 </sst>
 </file>
@@ -458,7 +461,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F5" sqref="F5:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,11 +569,11 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" t="str">
         <f>_xlfn.CONCAT("[InlineData(""",Tabela1[[#This Row],[Nome]],""",",Tabela1[[#This Row],[Idade]],", ",Tabela1[[#This Row],[ehCliente]],",""",Tabela1[[#This Row],[Resultado]],""")]")</f>
-        <v>[InlineData("João",18, true,"Argumento inválido")]</v>
+        <v>[InlineData("João",18, true,"Argumento inválido  (Parameter 'nome')")]</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -587,11 +590,11 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F6" t="str">
         <f>_xlfn.CONCAT("[InlineData(""",Tabela1[[#This Row],[Nome]],""",",Tabela1[[#This Row],[Idade]],", ",Tabela1[[#This Row],[ehCliente]],",""",Tabela1[[#This Row],[Resultado]],""")]")</f>
-        <v>[InlineData("1234 de oliveira 4",18, true,"Argumento inválido")]</v>
+        <v>[InlineData("1234 de oliveira 4",18, true,"Argumento inválido  (Parameter 'nome')")]</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -608,7 +611,7 @@
         <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F7" t="str">
         <f>_xlfn.CONCAT("[InlineData(""",Tabela1[[#This Row],[Nome]],""",",Tabela1[[#This Row],[Idade]],", ",Tabela1[[#This Row],[ehCliente]],",""",Tabela1[[#This Row],[Resultado]],""")]")</f>
@@ -629,11 +632,11 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F8" t="str">
         <f>_xlfn.CONCAT("[InlineData(""",Tabela1[[#This Row],[Nome]],""",",Tabela1[[#This Row],[Idade]],", ",Tabela1[[#This Row],[ehCliente]],",""",Tabela1[[#This Row],[Resultado]],""")]")</f>
-        <v>[InlineData("João Batista",0, true,"Argumento inválido")]</v>
+        <v>[InlineData("João Batista",0, true,"Argumento inválido  (Parameter 'idade')")]</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -650,11 +653,11 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F9" t="str">
         <f>_xlfn.CONCAT("[InlineData(""",Tabela1[[#This Row],[Nome]],""",",Tabela1[[#This Row],[Idade]],", ",Tabela1[[#This Row],[ehCliente]],",""",Tabela1[[#This Row],[Resultado]],""")]")</f>
-        <v>[InlineData("João Batista",121, true,"Argumento inválido")]</v>
+        <v>[InlineData("João Batista",121, true,"Argumento inválido  (Parameter 'idade')")]</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>